<commit_message>
upload USGS ShakeMap grid and uncertainty files
</commit_message>
<xml_diff>
--- a/testing_scenarios.xlsx
+++ b/testing_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_scenario_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E82483F-32E1-E74A-A213-AB1A242773D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE93C5E-A633-FE49-9676-B656367396FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="27480" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="272">
   <si>
     <t>Date</t>
   </si>
@@ -1150,9 +1150,6 @@
   </si>
   <si>
     <t>Total Damages ($M)</t>
-  </si>
-  <si>
-    <t>www-emdat.be</t>
   </si>
   <si>
     <t>References</t>
@@ -1238,6 +1235,9 @@
   </si>
   <si>
     <t>Exposure_Time</t>
+  </si>
+  <si>
+    <t>www.emdat.be</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1631,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1701,7 +1701,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2241,11 +2240,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J49" sqref="J49"/>
+      <selection pane="bottomRight" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2266,7 @@
     <col min="21" max="21" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="20.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="73" customWidth="1"/>
     <col min="26" max="27" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
@@ -2278,53 +2277,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="8" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="51" t="s">
+      <c r="A1" s="44"/>
+      <c r="B1" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="49"/>
-      <c r="AF1" s="50"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="49"/>
       <c r="AG1" s="32"/>
     </row>
     <row r="2" spans="1:36" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>251</v>
+      <c r="B2" s="42" t="s">
+        <v>250</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>0</v>
@@ -2369,10 +2368,10 @@
         <v>98</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T2" s="33" t="s">
         <v>203</v>
@@ -2399,7 +2398,7 @@
         <v>200</v>
       </c>
       <c r="AB2" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AC2" s="33" t="s">
         <v>204</v>
@@ -2418,14 +2417,14 @@
       </c>
     </row>
     <row r="3" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>52</v>
@@ -2501,7 +2500,7 @@
         <v>20000</v>
       </c>
       <c r="AG3" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2512,7 +2511,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>16</v>
@@ -2594,7 +2593,7 @@
         <v>900</v>
       </c>
       <c r="AG4" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2605,7 +2604,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>18</v>
@@ -2678,7 +2677,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>20</v>
@@ -2758,7 +2757,7 @@
         <v>745</v>
       </c>
       <c r="AG6" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2769,7 +2768,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>30</v>
@@ -2841,7 +2840,7 @@
       </c>
       <c r="AF7" s="34"/>
       <c r="AG7" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2852,7 +2851,7 @@
         <v>72</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>73</v>
@@ -2932,7 +2931,7 @@
       </c>
       <c r="AF8" s="34"/>
       <c r="AG8" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2943,7 +2942,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>75</v>
@@ -3016,7 +3015,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>66</v>
@@ -3098,7 +3097,7 @@
         <v>500</v>
       </c>
       <c r="AG10" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3109,7 +3108,7 @@
         <v>84</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>85</v>
@@ -3195,7 +3194,7 @@
         <v>750</v>
       </c>
       <c r="AG11" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3206,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>11</v>
@@ -3280,7 +3279,7 @@
         <v>50</v>
       </c>
       <c r="AG12" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3291,7 +3290,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>11</v>
@@ -3365,7 +3364,7 @@
       <c r="AE13" s="34"/>
       <c r="AF13" s="34"/>
       <c r="AG13" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3376,7 +3375,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>24</v>
@@ -3456,7 +3455,7 @@
         <v>450</v>
       </c>
       <c r="AG14" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3467,7 +3466,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>22</v>
@@ -3551,7 +3550,7 @@
         <v>422.7</v>
       </c>
       <c r="AG15" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
@@ -3565,7 +3564,7 @@
         <v>90</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>91</v>
@@ -3649,7 +3648,7 @@
         <v>205.8</v>
       </c>
       <c r="AG16" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -3663,7 +3662,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>7</v>
@@ -3748,7 +3747,7 @@
         <v>146</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>147</v>
@@ -3834,7 +3833,7 @@
         <v>4524.8999999999996</v>
       </c>
       <c r="AG18" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3845,7 +3844,7 @@
         <v>57</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>58</v>
@@ -3918,7 +3917,7 @@
         <v>160</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>161</v>
@@ -3981,9 +3980,7 @@
       <c r="AD20" s="34"/>
       <c r="AE20" s="34"/>
       <c r="AF20" s="34"/>
-      <c r="AG20" s="36" t="s">
-        <v>243</v>
-      </c>
+      <c r="AG20" s="36"/>
     </row>
     <row r="21" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
@@ -3993,7 +3990,7 @@
         <v>86</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>87</v>
@@ -4077,7 +4074,7 @@
         <v>550</v>
       </c>
       <c r="AG21" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4088,7 +4085,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>81</v>
@@ -4176,21 +4173,21 @@
         <v>20000</v>
       </c>
       <c r="AG22" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
     <row r="23" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="11" t="s">
         <v>182</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>13</v>
@@ -4274,7 +4271,7 @@
         <v>4200</v>
       </c>
       <c r="AG23" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4285,7 +4282,7 @@
         <v>88</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>89</v>
@@ -4369,7 +4366,7 @@
         <v>1000</v>
       </c>
       <c r="AG24" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4380,7 +4377,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>40</v>
@@ -4458,7 +4455,7 @@
         <v>12</v>
       </c>
       <c r="AG25" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4469,7 +4466,7 @@
         <v>41</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>42</v>
@@ -4548,7 +4545,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>62</v>
@@ -4630,7 +4627,7 @@
         <v>796</v>
       </c>
       <c r="AG27" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4641,7 +4638,7 @@
         <v>63</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>64</v>
@@ -4707,7 +4704,7 @@
       <c r="AE28" s="34"/>
       <c r="AF28" s="34"/>
       <c r="AG28" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
@@ -4721,7 +4718,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>68</v>
@@ -4801,7 +4798,7 @@
         <v>35</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>36</v>
@@ -4878,7 +4875,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>48</v>
@@ -4964,7 +4961,7 @@
         <v>2500</v>
       </c>
       <c r="AG31" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4975,7 +4972,7 @@
         <v>49</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>50</v>
@@ -5052,7 +5049,7 @@
         <v>76</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>77</v>
@@ -5136,7 +5133,7 @@
         <v>132.26</v>
       </c>
       <c r="AG33" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5147,7 +5144,7 @@
         <v>82</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>83</v>
@@ -5235,7 +5232,7 @@
         <v>1500</v>
       </c>
       <c r="AG34" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5246,7 +5243,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>44</v>
@@ -5326,7 +5323,7 @@
         <v>15800</v>
       </c>
       <c r="AG35" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5337,7 +5334,7 @@
         <v>45</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>46</v>
@@ -5411,7 +5408,7 @@
       </c>
       <c r="AF36" s="34"/>
       <c r="AG36" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5422,7 +5419,7 @@
         <v>25</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>26</v>
@@ -5498,7 +5495,7 @@
         <v>178</v>
       </c>
       <c r="AG37" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5509,7 +5506,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>28</v>
@@ -5586,7 +5583,7 @@
         <v>31</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>32</v>
@@ -5667,7 +5664,7 @@
         <v>78</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>79</v>
@@ -5743,7 +5740,7 @@
         <v>200</v>
       </c>
       <c r="AG40" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5754,7 +5751,7 @@
         <v>59</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>60</v>
@@ -5836,7 +5833,7 @@
         <v>5000</v>
       </c>
       <c r="AG41" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5847,7 +5844,7 @@
         <v>53</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>54</v>
@@ -5882,7 +5879,7 @@
       <c r="N42" s="14">
         <v>1.2</v>
       </c>
-      <c r="O42" s="47">
+      <c r="O42" s="46">
         <v>9.2355</v>
       </c>
       <c r="P42" s="14" t="s">
@@ -5919,7 +5916,7 @@
         <v>200</v>
       </c>
       <c r="AG42" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="43" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5930,7 +5927,7 @@
         <v>55</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>56</v>
@@ -6008,7 +6005,7 @@
         <v>200</v>
       </c>
       <c r="AG43" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6019,7 +6016,7 @@
         <v>69</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>70</v>
@@ -6054,7 +6051,7 @@
       <c r="N44" s="14">
         <v>0</v>
       </c>
-      <c r="O44" s="47">
+      <c r="O44" s="46">
         <v>12.411</v>
       </c>
       <c r="P44" s="14" t="s">
@@ -6101,7 +6098,7 @@
         <v>18</v>
       </c>
       <c r="AG44" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6112,7 +6109,7 @@
         <v>33</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>34</v>
@@ -6192,7 +6189,7 @@
       <c r="AE45" s="34"/>
       <c r="AF45" s="34"/>
       <c r="AG45" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.2">
@@ -6203,7 +6200,7 @@
         <v>93</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>92</v>
@@ -6287,21 +6284,21 @@
         <v>700</v>
       </c>
       <c r="AG46" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>253</v>
-      </c>
       <c r="C47" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>2</v>
@@ -6364,7 +6361,7 @@
         <v>1800</v>
       </c>
       <c r="Y47" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Z47" s="34">
         <v>1</v>
@@ -6386,21 +6383,21 @@
         <v>6800</v>
       </c>
       <c r="AG47" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B48" s="13" t="s">
-        <v>256</v>
-      </c>
       <c r="C48" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>269</v>
+        <v>263</v>
+      </c>
+      <c r="D48" s="41" t="s">
+        <v>268</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>2</v>
@@ -6439,7 +6436,7 @@
         <v>132</v>
       </c>
       <c r="Q48" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R48" s="14" t="s">
         <v>5</v>
@@ -6463,7 +6460,7 @@
         <v>1000</v>
       </c>
       <c r="Y48" s="34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z48" s="34">
         <v>8</v>
@@ -6481,21 +6478,21 @@
         <v>469.44400000000002</v>
       </c>
       <c r="AG48" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="B49" s="13" t="s">
-        <v>259</v>
-      </c>
       <c r="C49" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>14</v>
@@ -6534,7 +6531,7 @@
         <v>132</v>
       </c>
       <c r="Q49" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="R49" s="14" t="s">
         <v>5</v>
@@ -6554,7 +6551,7 @@
         <v>400</v>
       </c>
       <c r="Y49" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Z49" s="34">
         <v>115</v>
@@ -6574,21 +6571,21 @@
         <v>450</v>
       </c>
       <c r="AG49" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>14</v>
@@ -6627,7 +6624,7 @@
         <v>132</v>
       </c>
       <c r="Q50" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R50" s="14" t="s">
         <v>5</v>
@@ -6655,7 +6652,7 @@
       <c r="AE50" s="34"/>
       <c r="AF50" s="34"/>
       <c r="AG50" s="36" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6750,7 +6747,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -6850,12 +6847,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add CPI data from EM-DAT
</commit_message>
<xml_diff>
--- a/testing_scenarios.xlsx
+++ b/testing_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_scenario_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE93C5E-A633-FE49-9676-B656367396FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894F48BF-BAB4-0D40-AA77-1D7E2025CBCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="27480" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="273">
   <si>
     <t>Date</t>
   </si>
@@ -1238,6 +1238,9 @@
   </si>
   <si>
     <t>www.emdat.be</t>
+  </si>
+  <si>
+    <t>CPI</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1634,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1713,6 +1716,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2238,13 +2244,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ51"/>
+  <dimension ref="A1:AK51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AA22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB10" sqref="AB10"/>
+      <selection pane="bottomRight" activeCell="AF43" sqref="AF43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,49 +2279,51 @@
     <col min="30" max="30" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="20" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.5" customWidth="1"/>
+    <col min="33" max="33" width="18" customWidth="1"/>
+    <col min="34" max="34" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="8" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" s="8" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="44"/>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="47" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="49"/>
-      <c r="AG1" s="32"/>
-    </row>
-    <row r="2" spans="1:36" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="32"/>
+    </row>
+    <row r="2" spans="1:37" s="8" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
         <v>101</v>
       </c>
@@ -2413,10 +2421,13 @@
         <v>242</v>
       </c>
       <c r="AG2" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH2" s="33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>111</v>
       </c>
@@ -2499,11 +2510,14 @@
       <c r="AF3" s="34">
         <v>20000</v>
       </c>
-      <c r="AG3" s="36" t="s">
+      <c r="AG3" s="34">
+        <v>31.841106568786898</v>
+      </c>
+      <c r="AH3" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>190</v>
       </c>
@@ -2592,11 +2606,14 @@
       <c r="AF4" s="34">
         <v>900</v>
       </c>
-      <c r="AG4" s="36" t="s">
+      <c r="AG4" s="34">
+        <v>35.131791507319001</v>
+      </c>
+      <c r="AH4" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>191</v>
       </c>
@@ -2667,9 +2684,10 @@
       <c r="AD5" s="34"/>
       <c r="AE5" s="34"/>
       <c r="AF5" s="34"/>
-      <c r="AG5" s="36"/>
-    </row>
-    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="36"/>
+    </row>
+    <row r="6" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>102</v>
       </c>
@@ -2756,11 +2774,14 @@
       <c r="AF6" s="34">
         <v>745</v>
       </c>
-      <c r="AG6" s="36" t="s">
+      <c r="AG6" s="34">
+        <v>42.3506985655047</v>
+      </c>
+      <c r="AH6" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>105</v>
       </c>
@@ -2839,11 +2860,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AF7" s="34"/>
-      <c r="AG7" s="36" t="s">
+      <c r="AG7" s="34"/>
+      <c r="AH7" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>198</v>
       </c>
@@ -2930,11 +2952,12 @@
         <v>23.7</v>
       </c>
       <c r="AF8" s="34"/>
-      <c r="AG8" s="36" t="s">
+      <c r="AG8" s="34"/>
+      <c r="AH8" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>199</v>
       </c>
@@ -3005,9 +3028,10 @@
       <c r="AD9" s="34"/>
       <c r="AE9" s="34"/>
       <c r="AF9" s="34"/>
-      <c r="AG9" s="36"/>
-    </row>
-    <row r="10" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG9" s="34"/>
+      <c r="AH9" s="36"/>
+    </row>
+    <row r="10" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>113</v>
       </c>
@@ -3096,11 +3120,14 @@
       <c r="AF10" s="34">
         <v>500</v>
       </c>
-      <c r="AG10" s="36" t="s">
+      <c r="AG10" s="34">
+        <v>50.484032265154497</v>
+      </c>
+      <c r="AH10" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>119</v>
       </c>
@@ -3193,11 +3220,14 @@
       <c r="AF11" s="34">
         <v>750</v>
       </c>
-      <c r="AG11" s="36" t="s">
+      <c r="AG11" s="34">
+        <v>54.215844652512203</v>
+      </c>
+      <c r="AH11" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>181</v>
       </c>
@@ -3278,11 +3308,14 @@
       <c r="AF12" s="34">
         <v>50</v>
       </c>
-      <c r="AG12" s="36" t="s">
+      <c r="AG12" s="34">
+        <v>54.215844652512203</v>
+      </c>
+      <c r="AH12" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>128</v>
       </c>
@@ -3363,11 +3396,12 @@
       <c r="AD13" s="34"/>
       <c r="AE13" s="34"/>
       <c r="AF13" s="34"/>
-      <c r="AG13" s="36" t="s">
+      <c r="AG13" s="34"/>
+      <c r="AH13" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>104</v>
       </c>
@@ -3454,11 +3488,14 @@
       <c r="AF14" s="34">
         <v>450</v>
       </c>
-      <c r="AG14" s="36" t="s">
+      <c r="AG14" s="34">
+        <v>58.878183290107998</v>
+      </c>
+      <c r="AH14" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>103</v>
       </c>
@@ -3549,14 +3586,17 @@
       <c r="AF15" s="34">
         <v>422.7</v>
       </c>
-      <c r="AG15" s="36" t="s">
+      <c r="AG15" s="34">
+        <v>58.878183290107998</v>
+      </c>
+      <c r="AH15" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
-    </row>
-    <row r="16" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AK15" s="1"/>
+    </row>
+    <row r="16" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>185</v>
       </c>
@@ -3647,14 +3687,17 @@
       <c r="AF16" s="34">
         <v>205.8</v>
       </c>
-      <c r="AG16" s="36" t="s">
+      <c r="AG16" s="34">
+        <v>58.878183290107998</v>
+      </c>
+      <c r="AH16" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
-    </row>
-    <row r="17" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AK16" s="1"/>
+    </row>
+    <row r="17" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>183</v>
       </c>
@@ -3737,9 +3780,10 @@
       <c r="AD17" s="34"/>
       <c r="AE17" s="34"/>
       <c r="AF17" s="34"/>
-      <c r="AG17" s="36"/>
-    </row>
-    <row r="18" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG17" s="34"/>
+      <c r="AH17" s="36"/>
+    </row>
+    <row r="18" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>159</v>
       </c>
@@ -3832,11 +3876,14 @@
       <c r="AF18" s="34">
         <v>4524.8999999999996</v>
       </c>
-      <c r="AG18" s="36" t="s">
+      <c r="AG18" s="34">
+        <v>62.020757322666199</v>
+      </c>
+      <c r="AH18" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>145</v>
       </c>
@@ -3907,9 +3954,10 @@
       <c r="AD19" s="34"/>
       <c r="AE19" s="34"/>
       <c r="AF19" s="34"/>
-      <c r="AG19" s="36"/>
-    </row>
-    <row r="20" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG19" s="34"/>
+      <c r="AH19" s="36"/>
+    </row>
+    <row r="20" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>180</v>
       </c>
@@ -3980,9 +4028,10 @@
       <c r="AD20" s="34"/>
       <c r="AE20" s="34"/>
       <c r="AF20" s="34"/>
-      <c r="AG20" s="36"/>
-    </row>
-    <row r="21" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG20" s="34"/>
+      <c r="AH20" s="36"/>
+    </row>
+    <row r="21" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>120</v>
       </c>
@@ -4073,11 +4122,14 @@
       <c r="AF21" s="34">
         <v>550</v>
       </c>
-      <c r="AG21" s="36" t="s">
+      <c r="AG21" s="34">
+        <v>62.983501106275703</v>
+      </c>
+      <c r="AH21" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="22" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>117</v>
       </c>
@@ -4172,14 +4224,17 @@
       <c r="AF22" s="34">
         <v>20000</v>
       </c>
-      <c r="AG22" s="36" t="s">
+      <c r="AG22" s="34">
+        <v>64.361592817266697</v>
+      </c>
+      <c r="AH22" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
-    </row>
-    <row r="23" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AK22" s="1"/>
+    </row>
+    <row r="23" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>182</v>
       </c>
@@ -4270,11 +4325,14 @@
       <c r="AF23" s="34">
         <v>4200</v>
       </c>
-      <c r="AG23" s="36" t="s">
+      <c r="AG23" s="34">
+        <v>64.361592817266697</v>
+      </c>
+      <c r="AH23" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="24" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>121</v>
       </c>
@@ -4365,11 +4423,14 @@
       <c r="AF24" s="34">
         <v>1000</v>
       </c>
-      <c r="AG24" s="36" t="s">
+      <c r="AG24" s="34">
+        <v>64.361592817266697</v>
+      </c>
+      <c r="AH24" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>109</v>
       </c>
@@ -4454,11 +4515,14 @@
       <c r="AF25" s="34">
         <v>12</v>
       </c>
-      <c r="AG25" s="36" t="s">
+      <c r="AG25" s="34">
+        <v>66.534994212199805</v>
+      </c>
+      <c r="AH25" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>110</v>
       </c>
@@ -4535,9 +4599,10 @@
       <c r="AD26" s="34"/>
       <c r="AE26" s="34"/>
       <c r="AF26" s="34"/>
-      <c r="AG26" s="36"/>
-    </row>
-    <row r="27" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG26" s="34"/>
+      <c r="AH26" s="36"/>
+    </row>
+    <row r="27" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>186</v>
       </c>
@@ -4626,11 +4691,14 @@
       <c r="AF27" s="34">
         <v>796</v>
       </c>
-      <c r="AG27" s="36" t="s">
+      <c r="AG27" s="34">
+        <v>69.500472548243906</v>
+      </c>
+      <c r="AH27" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="28" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>187</v>
       </c>
@@ -4703,14 +4771,15 @@
       <c r="AD28" s="34"/>
       <c r="AE28" s="34"/>
       <c r="AF28" s="34"/>
-      <c r="AG28" s="36" t="s">
+      <c r="AG28" s="34"/>
+      <c r="AH28" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
-    </row>
-    <row r="29" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AK28" s="1"/>
+    </row>
+    <row r="29" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>114</v>
       </c>
@@ -4785,12 +4854,13 @@
       <c r="AD29" s="34"/>
       <c r="AE29" s="34"/>
       <c r="AF29" s="34"/>
-      <c r="AG29" s="36"/>
-      <c r="AH29" s="1"/>
+      <c r="AG29" s="34"/>
+      <c r="AH29" s="36"/>
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
-    </row>
-    <row r="30" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AK29" s="1"/>
+    </row>
+    <row r="30" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>108</v>
       </c>
@@ -4865,9 +4935,10 @@
       <c r="AD30" s="34"/>
       <c r="AE30" s="34"/>
       <c r="AF30" s="34"/>
-      <c r="AG30" s="36"/>
-    </row>
-    <row r="31" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG30" s="34"/>
+      <c r="AH30" s="36"/>
+    </row>
+    <row r="31" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>194</v>
       </c>
@@ -4960,11 +5031,14 @@
       <c r="AF31" s="34">
         <v>2500</v>
       </c>
-      <c r="AG31" s="36" t="s">
+      <c r="AG31" s="34">
+        <v>82.893249886441893</v>
+      </c>
+      <c r="AH31" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="32" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>195</v>
       </c>
@@ -5039,9 +5113,10 @@
       <c r="AD32" s="34"/>
       <c r="AE32" s="34"/>
       <c r="AF32" s="34"/>
-      <c r="AG32" s="36"/>
-    </row>
-    <row r="33" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG32" s="34"/>
+      <c r="AH32" s="36"/>
+    </row>
+    <row r="33" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>184</v>
       </c>
@@ -5132,11 +5207,14 @@
       <c r="AF33" s="34">
         <v>132.26</v>
       </c>
-      <c r="AG33" s="36" t="s">
+      <c r="AG33" s="34">
+        <v>84.252732720852194</v>
+      </c>
+      <c r="AH33" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>118</v>
       </c>
@@ -5231,11 +5309,14 @@
       <c r="AF34" s="34">
         <v>1500</v>
       </c>
-      <c r="AG34" s="36" t="s">
+      <c r="AG34" s="34">
+        <v>86.912465016777304</v>
+      </c>
+      <c r="AH34" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>192</v>
       </c>
@@ -5322,11 +5403,14 @@
       <c r="AF35" s="34">
         <v>15800</v>
       </c>
-      <c r="AG35" s="36" t="s">
+      <c r="AG35" s="34">
+        <v>88.710968980321496</v>
+      </c>
+      <c r="AH35" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="36" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>193</v>
       </c>
@@ -5407,11 +5491,12 @@
         <v>1300</v>
       </c>
       <c r="AF36" s="34"/>
-      <c r="AG36" s="36" t="s">
+      <c r="AG36" s="34"/>
+      <c r="AH36" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="37" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>188</v>
       </c>
@@ -5494,11 +5579,14 @@
       <c r="AF37" s="34">
         <v>178</v>
       </c>
-      <c r="AG37" s="36" t="s">
+      <c r="AG37" s="34">
+        <v>91.470614092927207</v>
+      </c>
+      <c r="AH37" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="38" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>189</v>
       </c>
@@ -5573,9 +5661,10 @@
       <c r="AD38" s="34"/>
       <c r="AE38" s="34"/>
       <c r="AF38" s="34"/>
-      <c r="AG38" s="36"/>
-    </row>
-    <row r="39" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG38" s="34"/>
+      <c r="AH38" s="36"/>
+    </row>
+    <row r="39" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>106</v>
       </c>
@@ -5654,9 +5743,10 @@
       <c r="AD39" s="34"/>
       <c r="AE39" s="34"/>
       <c r="AF39" s="34"/>
-      <c r="AG39" s="36"/>
-    </row>
-    <row r="40" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG39" s="34"/>
+      <c r="AH39" s="36"/>
+    </row>
+    <row r="40" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>116</v>
       </c>
@@ -5720,30 +5810,17 @@
       <c r="W40" s="34"/>
       <c r="X40" s="34"/>
       <c r="Y40" s="36"/>
-      <c r="Z40" s="34">
-        <v>10</v>
-      </c>
-      <c r="AA40" s="34">
-        <v>300</v>
-      </c>
-      <c r="AB40" s="34">
-        <v>15000</v>
-      </c>
-      <c r="AC40" s="34">
-        <v>15300</v>
-      </c>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="34"/>
+      <c r="AC40" s="34"/>
       <c r="AD40" s="34"/>
-      <c r="AE40" s="34">
-        <v>100</v>
-      </c>
-      <c r="AF40" s="34">
-        <v>200</v>
-      </c>
-      <c r="AG40" s="36" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="41" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE40" s="34"/>
+      <c r="AF40" s="34"/>
+      <c r="AG40" s="34"/>
+      <c r="AH40" s="36"/>
+    </row>
+    <row r="41" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>112</v>
       </c>
@@ -5832,11 +5909,14 @@
       <c r="AF41" s="34">
         <v>5000</v>
       </c>
-      <c r="AG41" s="36" t="s">
+      <c r="AG41" s="34">
+        <v>92.734479171245596</v>
+      </c>
+      <c r="AH41" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>196</v>
       </c>
@@ -5915,11 +5995,14 @@
       <c r="AF42" s="34">
         <v>200</v>
       </c>
-      <c r="AG42" s="36" t="s">
+      <c r="AG42" s="34">
+        <v>92.734479171245596</v>
+      </c>
+      <c r="AH42" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>197</v>
       </c>
@@ -6004,11 +6087,14 @@
       <c r="AF43" s="34">
         <v>200</v>
       </c>
-      <c r="AG43" s="36" t="s">
+      <c r="AG43" s="34">
+        <v>92.734479171245596</v>
+      </c>
+      <c r="AH43" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>115</v>
       </c>
@@ -6097,11 +6183,14 @@
       <c r="AF44" s="34">
         <v>18</v>
       </c>
-      <c r="AG44" s="36" t="s">
+      <c r="AG44" s="34">
+        <v>94.709840725599705</v>
+      </c>
+      <c r="AH44" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="45" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>107</v>
       </c>
@@ -6188,11 +6277,12 @@
       <c r="AD45" s="34"/>
       <c r="AE45" s="34"/>
       <c r="AF45" s="34"/>
-      <c r="AG45" s="36" t="s">
+      <c r="AG45" s="34"/>
+      <c r="AH45" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="37" t="s">
         <v>122</v>
       </c>
@@ -6283,11 +6373,14 @@
       <c r="AF46" s="34">
         <v>700</v>
       </c>
-      <c r="AG46" s="36" t="s">
+      <c r="AG46" s="34">
+        <v>98.781448268788395</v>
+      </c>
+      <c r="AH46" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>251</v>
       </c>
@@ -6382,11 +6475,14 @@
       <c r="AF47" s="34">
         <v>6800</v>
       </c>
-      <c r="AG47" s="36" t="s">
+      <c r="AG47" s="34">
+        <v>100</v>
+      </c>
+      <c r="AH47" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>254</v>
       </c>
@@ -6477,11 +6573,14 @@
       <c r="AF48" s="34">
         <v>469.44400000000002</v>
       </c>
-      <c r="AG48" s="36" t="s">
+      <c r="AG48" s="34">
+        <v>100</v>
+      </c>
+      <c r="AH48" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>257</v>
       </c>
@@ -6570,11 +6669,14 @@
       <c r="AF49" s="34">
         <v>450</v>
       </c>
-      <c r="AG49" s="36" t="s">
+      <c r="AG49" s="34">
+        <v>100</v>
+      </c>
+      <c r="AH49" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>260</v>
       </c>
@@ -6651,11 +6753,12 @@
       <c r="AD50" s="34"/>
       <c r="AE50" s="34"/>
       <c r="AF50" s="34"/>
-      <c r="AG50" s="36" t="s">
+      <c r="AG50" s="34"/>
+      <c r="AH50" s="36" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>124</v>
       </c>
@@ -6715,10 +6818,11 @@
       <c r="AE51" s="34"/>
       <c r="AF51" s="34"/>
       <c r="AG51" s="34"/>
+      <c r="AH51" s="34"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:S51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState ref="A3:AG52">
+  <sortState ref="A3:AH52">
     <sortCondition ref="D3"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>